<commit_message>
Remove interactive XML generation script and associated output file to streamline the EUDAMED XML generation process.
</commit_message>
<xml_diff>
--- a/MC Data/Eudamed data structure filled 877PAY_clean.xlsx
+++ b/MC Data/Eudamed data structure filled 877PAY_clean.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\PMO Projects\24_01_E New ERP Introduction\Migration\EUDAMED\MC Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1FB479D3-BF83-4AA9-A2C3-61E9BD0C6EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A627E5C3-328B-431C-BEBD-D6742A5B7BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-1810" windowWidth="38620" windowHeight="21100" firstSheet="1" xr2:uid="{5DF1A440-2648-490F-B867-8F39A17616C4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24196" windowHeight="14476" xr2:uid="{5DF1A440-2648-490F-B867-8F39A17616C4}"/>
   </bookViews>
   <sheets>
     <sheet name="Structure" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
     <author>tc={1CD0303A-761E-4078-80D5-AD23DB6AB5DC}</author>
   </authors>
   <commentList>
-    <comment ref="D16" authorId="0" shapeId="0" xr:uid="{8A5B2ABB-581E-4D09-B939-F5D82E1FEA62}">
+    <comment ref="E16" authorId="0" shapeId="0" xr:uid="{8A5B2ABB-581E-4D09-B939-F5D82E1FEA62}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -70,7 +70,7 @@
     Ez változni fog idén nyáron 2265-re</t>
       </text>
     </comment>
-    <comment ref="D21" authorId="1" shapeId="0" xr:uid="{F572E940-087F-4354-9D1A-A24371C56133}">
+    <comment ref="E21" authorId="1" shapeId="0" xr:uid="{F572E940-087F-4354-9D1A-A24371C56133}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -82,7 +82,7 @@
     Fontos: GTIN14-et kell megadni</t>
       </text>
     </comment>
-    <comment ref="E23" authorId="2" shapeId="0" xr:uid="{8B519938-3E6C-4FF5-8FB0-FCB1CE70254F}">
+    <comment ref="F23" authorId="2" shapeId="0" xr:uid="{8B519938-3E6C-4FF5-8FB0-FCB1CE70254F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -92,7 +92,7 @@
     Double check Krisztivel</t>
       </text>
     </comment>
-    <comment ref="B24" authorId="3" shapeId="0" xr:uid="{4FCC3559-93FC-431F-896E-2BD675F86DB5}">
+    <comment ref="C24" authorId="3" shapeId="0" xr:uid="{4FCC3559-93FC-431F-896E-2BD675F86DB5}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -100,7 +100,7 @@
     DoC vagy Name: Posterior chamber...</t>
       </text>
     </comment>
-    <comment ref="B25" authorId="4" shapeId="0" xr:uid="{9277BFAF-88E7-4494-83C2-96C4A9D13A6A}">
+    <comment ref="C25" authorId="4" shapeId="0" xr:uid="{9277BFAF-88E7-4494-83C2-96C4A9D13A6A}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -108,7 +108,7 @@
     DoC vagy Name: Posterior chamber...</t>
       </text>
     </comment>
-    <comment ref="B26" authorId="5" shapeId="0" xr:uid="{24032FC1-03E6-4019-AA0D-D39C2F33047B}">
+    <comment ref="C26" authorId="5" shapeId="0" xr:uid="{24032FC1-03E6-4019-AA0D-D39C2F33047B}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -116,7 +116,7 @@
     DoC vagy Name: Posterior chamber...</t>
       </text>
     </comment>
-    <comment ref="B27" authorId="6" shapeId="0" xr:uid="{047C5054-E8D3-41E7-8A48-B8189E7C374C}">
+    <comment ref="C27" authorId="6" shapeId="0" xr:uid="{047C5054-E8D3-41E7-8A48-B8189E7C374C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -128,7 +128,7 @@
     Model name? (DoC)</t>
       </text>
     </comment>
-    <comment ref="D27" authorId="7" shapeId="0" xr:uid="{469B3B8C-9AAA-4F77-A9E0-627E46FBA57E}">
+    <comment ref="E27" authorId="7" shapeId="0" xr:uid="{469B3B8C-9AAA-4F77-A9E0-627E46FBA57E}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -140,7 +140,7 @@
     Fontos: GTIN14-et kell megadni</t>
       </text>
     </comment>
-    <comment ref="D30" authorId="8" shapeId="0" xr:uid="{CB3DD1A3-D70E-42C1-ADB5-EEDBE95CE57C}">
+    <comment ref="E30" authorId="8" shapeId="0" xr:uid="{CB3DD1A3-D70E-42C1-ADB5-EEDBE95CE57C}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -148,7 +148,7 @@
     SAP átállás után ez benne lesz, most nincsen.</t>
       </text>
     </comment>
-    <comment ref="D33" authorId="9" shapeId="0" xr:uid="{65BEF406-0A3A-492F-B3B3-522C2928A9AB}">
+    <comment ref="E33" authorId="9" shapeId="0" xr:uid="{65BEF406-0A3A-492F-B3B3-522C2928A9AB}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -156,7 +156,7 @@
     Kell?</t>
       </text>
     </comment>
-    <comment ref="B35" authorId="10" shapeId="0" xr:uid="{6B834A1C-93CE-42EF-B41A-A29ECFCE1F82}">
+    <comment ref="C35" authorId="10" shapeId="0" xr:uid="{6B834A1C-93CE-42EF-B41A-A29ECFCE1F82}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -164,7 +164,7 @@
     Mi a cél?</t>
       </text>
     </comment>
-    <comment ref="D35" authorId="11" shapeId="0" xr:uid="{07A9BCA0-A72F-45C0-9B30-3977D6F97AFC}">
+    <comment ref="E35" authorId="11" shapeId="0" xr:uid="{07A9BCA0-A72F-45C0-9B30-3977D6F97AFC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -172,7 +172,7 @@
     Mit adjunk meg? Teljes átmérő.</t>
       </text>
     </comment>
-    <comment ref="E35" authorId="12" shapeId="0" xr:uid="{29D4DEDB-FEEE-47A0-AAFF-D033EAC89026}">
+    <comment ref="F35" authorId="12" shapeId="0" xr:uid="{29D4DEDB-FEEE-47A0-AAFF-D033EAC89026}">
       <text>
         <t xml:space="preserve">[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -194,7 +194,7 @@
 </t>
       </text>
     </comment>
-    <comment ref="B48" authorId="13" shapeId="0" xr:uid="{B43E464E-5726-409D-A086-823698CBB3C2}">
+    <comment ref="C48" authorId="13" shapeId="0" xr:uid="{B43E464E-5726-409D-A086-823698CBB3C2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -204,7 +204,7 @@
     Lencséknél no, biovis, medjet, jetring</t>
       </text>
     </comment>
-    <comment ref="B49" authorId="14" shapeId="0" xr:uid="{9D76ACBD-4553-4AD1-8506-A5BB74A2FDA2}">
+    <comment ref="C49" authorId="14" shapeId="0" xr:uid="{9D76ACBD-4553-4AD1-8506-A5BB74A2FDA2}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -214,7 +214,7 @@
     PMCF clinical investigation is ide tartozik? Ha nem, akkor nem. Kérdező felület, Eudamed?</t>
       </text>
     </comment>
-    <comment ref="B54" authorId="15" shapeId="0" xr:uid="{E14E57AC-D0A2-4625-9716-153B4C796039}">
+    <comment ref="C54" authorId="15" shapeId="0" xr:uid="{E14E57AC-D0A2-4625-9716-153B4C796039}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -226,7 +226,7 @@
     Első CE certification?</t>
       </text>
     </comment>
-    <comment ref="D55" authorId="16" shapeId="0" xr:uid="{1CD0303A-761E-4078-80D5-AD23DB6AB5DC}">
+    <comment ref="E55" authorId="16" shapeId="0" xr:uid="{1CD0303A-761E-4078-80D5-AD23DB6AB5DC}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2294" uniqueCount="490">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2325" uniqueCount="521">
   <si>
     <t>Topic</t>
   </si>
@@ -2044,6 +2044,99 @@
   </si>
   <si>
     <t>BioVis 3.0%</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/riskClass</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/modelName</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/modelName/name</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/identifier/DICode</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/identifier/issuingEntityCode</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/animalTissuesCells</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/humanTissuesCells</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/humanProductCheck</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/medicinalProductCheck</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/active</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/administeringMedicine</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/implantable</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/measuringFunction</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/reusable</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/identifier/DICode</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/identifier/issuingEntityCode</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/status/code</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/MDNCodes</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/referenceNumber</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/sterile</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/sterilization</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/latex</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/reprocessed</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRBasicUDI/type</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/tradeNames/name/textValue</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/baseQuantity</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/productionIdentifier</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/website</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/criticalWarnings/warning/comments/name/textValue</t>
+  </si>
+  <si>
+    <t>MDRDevice/MDRUDIDIData/storageHandlingConditions/condition/storageHandlingConditionValue</t>
+  </si>
+  <si>
+    <t>XMLPath</t>
   </si>
 </sst>
 </file>
@@ -2189,9 +2282,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
       <family val="2"/>
       <charset val="238"/>
     </font>
@@ -2250,7 +2343,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2326,16 +2419,22 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="12">
     <dxf>
-      <font>
-        <b/>
-      </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2360,6 +2459,29 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <charset val="238"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="1" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -2406,18 +2528,19 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{360A8FDE-19FF-40FB-BC4A-F271D69A7631}" name="Table1" displayName="Table1" ref="A1:I57" totalsRowShown="0" headerRowDxfId="10" dataDxfId="9">
-  <autoFilter ref="A1:I57" xr:uid="{360A8FDE-19FF-40FB-BC4A-F271D69A7631}"/>
-  <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{E7EF6E43-A89E-42AD-BEE6-4F1A89D2984E}" name="Topic" dataDxfId="0"/>
-    <tableColumn id="2" xr3:uid="{C34AA74D-EA58-4902-91F3-764B3B53FF7E}" name="Question" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{6D6D93FC-487E-468B-A809-E2E695EC6C71}" name="Subquestion" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{EA675C2D-1F8A-4940-8092-D4D23D2F9D69}" name="Answer1" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{9A2B6F93-2678-423B-AF23-A041B9CC58A8}" name="Answer2" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{CA736CD0-C2E3-427B-AC94-AAAAE8A0BBA6}" name="Answer3" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{34F60157-F725-49D9-BE40-946730DEC7C0}" name="Answer4" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{B07DC268-F625-4F9A-897F-9C9A3C921209}" name="Answer5" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{6D75A019-C9EB-4DC3-A5A4-74821447C4A1}" name="Answer6" dataDxfId="2"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{360A8FDE-19FF-40FB-BC4A-F271D69A7631}" name="Table1" displayName="Table1" ref="A1:J57" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <autoFilter ref="A1:J57" xr:uid="{360A8FDE-19FF-40FB-BC4A-F271D69A7631}"/>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{E7EF6E43-A89E-42AD-BEE6-4F1A89D2984E}" name="Topic" dataDxfId="9"/>
+    <tableColumn id="10" xr3:uid="{7CDD16A9-21E5-4512-A417-ADF1DCB8FD80}" name="XMLPath" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{C34AA74D-EA58-4902-91F3-764B3B53FF7E}" name="Question" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{6D6D93FC-487E-468B-A809-E2E695EC6C71}" name="Subquestion" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{EA675C2D-1F8A-4940-8092-D4D23D2F9D69}" name="Answer1" dataDxfId="5"/>
+    <tableColumn id="5" xr3:uid="{9A2B6F93-2678-423B-AF23-A041B9CC58A8}" name="Answer2" dataDxfId="4"/>
+    <tableColumn id="6" xr3:uid="{CA736CD0-C2E3-427B-AC94-AAAAE8A0BBA6}" name="Answer3" dataDxfId="3"/>
+    <tableColumn id="7" xr3:uid="{34F60157-F725-49D9-BE40-946730DEC7C0}" name="Answer4" dataDxfId="2"/>
+    <tableColumn id="8" xr3:uid="{B07DC268-F625-4F9A-897F-9C9A3C921209}" name="Answer5" dataDxfId="1"/>
+    <tableColumn id="9" xr3:uid="{6D75A019-C9EB-4DC3-A5A4-74821447C4A1}" name="Answer6" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2720,64 +2843,64 @@
 
 <file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
 <ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <threadedComment ref="D16" dT="2025-03-13T14:32:40.87" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{8A5B2ABB-581E-4D09-B939-F5D82E1FEA62}">
+  <threadedComment ref="E16" dT="2025-03-13T14:32:40.87" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{8A5B2ABB-581E-4D09-B939-F5D82E1FEA62}">
     <text>Ez változni fog idén nyáron 2265-re</text>
   </threadedComment>
-  <threadedComment ref="D21" dT="2025-03-13T15:51:41.12" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{F572E940-087F-4354-9D1A-A24371C56133}">
+  <threadedComment ref="E21" dT="2025-03-13T15:51:41.12" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{F572E940-087F-4354-9D1A-A24371C56133}">
     <text>LK-877PAYP020P2-EK0</text>
   </threadedComment>
-  <threadedComment ref="D21" dT="2025-03-13T15:52:14.57" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{23BDE3CE-C095-4165-AEA4-DEE320FF1309}" parentId="{F572E940-087F-4354-9D1A-A24371C56133}">
+  <threadedComment ref="E21" dT="2025-03-13T15:52:14.57" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{23BDE3CE-C095-4165-AEA4-DEE320FF1309}" parentId="{F572E940-087F-4354-9D1A-A24371C56133}">
     <text>Itt lesz a probléma, hiszen rengeteg GTIN számunk van: dioptria, cyl, csom.kód</text>
   </threadedComment>
-  <threadedComment ref="D21" dT="2025-03-14T11:42:05.89" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{5779F309-70E2-4F28-9F4D-7D5A012F4EF2}" parentId="{F572E940-087F-4354-9D1A-A24371C56133}">
+  <threadedComment ref="E21" dT="2025-03-14T11:42:05.89" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{5779F309-70E2-4F28-9F4D-7D5A012F4EF2}" parentId="{F572E940-087F-4354-9D1A-A24371C56133}">
     <text>Fontos: GTIN14-et kell megadni</text>
   </threadedComment>
-  <threadedComment ref="E23" dT="2025-03-14T11:47:50.60" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{8B519938-3E6C-4FF5-8FB0-FCB1CE70254F}">
+  <threadedComment ref="F23" dT="2025-03-14T11:47:50.60" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{8B519938-3E6C-4FF5-8FB0-FCB1CE70254F}">
     <text>K:\PMO Projects\24_01_E New ERP Introduction\Subprojects\Gyártás\TPM\EUDAMED</text>
   </threadedComment>
-  <threadedComment ref="E23" dT="2025-03-17T08:47:08.92" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{61CFFC06-C204-43B8-B2EF-5D27787DFBFC}" parentId="{8B519938-3E6C-4FF5-8FB0-FCB1CE70254F}">
+  <threadedComment ref="F23" dT="2025-03-17T08:47:08.92" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{61CFFC06-C204-43B8-B2EF-5D27787DFBFC}" parentId="{8B519938-3E6C-4FF5-8FB0-FCB1CE70254F}">
     <text>Double check Krisztivel</text>
   </threadedComment>
-  <threadedComment ref="B24" dT="2025-03-13T15:58:19.43" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{4FCC3559-93FC-431F-896E-2BD675F86DB5}">
+  <threadedComment ref="C24" dT="2025-03-13T15:58:19.43" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{4FCC3559-93FC-431F-896E-2BD675F86DB5}">
     <text>DoC vagy Name: Posterior chamber...</text>
   </threadedComment>
-  <threadedComment ref="B25" dT="2025-03-13T15:58:19.43" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{9277BFAF-88E7-4494-83C2-96C4A9D13A6A}">
+  <threadedComment ref="C25" dT="2025-03-13T15:58:19.43" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{9277BFAF-88E7-4494-83C2-96C4A9D13A6A}">
     <text>DoC vagy Name: Posterior chamber...</text>
   </threadedComment>
-  <threadedComment ref="B26" dT="2025-03-13T15:58:19.43" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{24032FC1-03E6-4019-AA0D-D39C2F33047B}">
+  <threadedComment ref="C26" dT="2025-03-13T15:58:19.43" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{24032FC1-03E6-4019-AA0D-D39C2F33047B}">
     <text>DoC vagy Name: Posterior chamber...</text>
   </threadedComment>
-  <threadedComment ref="B27" dT="2024-07-22T12:02:44.43" personId="{0520337A-CFA7-4E40-9D95-6AE1712FCF47}" id="{047C5054-E8D3-41E7-8A48-B8189E7C374C}">
+  <threadedComment ref="C27" dT="2024-07-22T12:02:44.43" personId="{0520337A-CFA7-4E40-9D95-6AE1712FCF47}" id="{047C5054-E8D3-41E7-8A48-B8189E7C374C}">
     <text>GS1-et megkérdezni</text>
   </threadedComment>
-  <threadedComment ref="B27" dT="2024-07-22T12:04:52.53" personId="{0520337A-CFA7-4E40-9D95-6AE1712FCF47}" id="{CB05A60E-CDB1-4554-A9A5-1E02CC5BCE79}" parentId="{047C5054-E8D3-41E7-8A48-B8189E7C374C}">
+  <threadedComment ref="C27" dT="2024-07-22T12:04:52.53" personId="{0520337A-CFA7-4E40-9D95-6AE1712FCF47}" id="{CB05A60E-CDB1-4554-A9A5-1E02CC5BCE79}" parentId="{047C5054-E8D3-41E7-8A48-B8189E7C374C}">
     <text>Kereszthivatkozás alkalmazása?!</text>
   </threadedComment>
-  <threadedComment ref="B27" dT="2025-03-07T13:18:01.90" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{31063EC4-1747-4841-8CB4-1D0947E669A7}" parentId="{047C5054-E8D3-41E7-8A48-B8189E7C374C}">
+  <threadedComment ref="C27" dT="2025-03-07T13:18:01.90" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{31063EC4-1747-4841-8CB4-1D0947E669A7}" parentId="{047C5054-E8D3-41E7-8A48-B8189E7C374C}">
     <text>Model name? (DoC)</text>
   </threadedComment>
-  <threadedComment ref="D27" dT="2025-03-13T15:51:41.12" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{469B3B8C-9AAA-4F77-A9E0-627E46FBA57E}">
+  <threadedComment ref="E27" dT="2025-03-13T15:51:41.12" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{469B3B8C-9AAA-4F77-A9E0-627E46FBA57E}">
     <text>LK-877PAYP020P2-EK0</text>
   </threadedComment>
-  <threadedComment ref="D27" dT="2025-03-13T15:52:14.57" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{11601174-721C-4DEF-8938-9AACBEAA1217}" parentId="{469B3B8C-9AAA-4F77-A9E0-627E46FBA57E}">
+  <threadedComment ref="E27" dT="2025-03-13T15:52:14.57" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{11601174-721C-4DEF-8938-9AACBEAA1217}" parentId="{469B3B8C-9AAA-4F77-A9E0-627E46FBA57E}">
     <text>Itt lesz a probléma, hiszen rengeteg GTIN számunk van: dioptria, cyl, csom.kód</text>
   </threadedComment>
-  <threadedComment ref="D27" dT="2025-03-14T11:42:05.89" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{C7EE2D89-B73E-4A20-A7C5-2FA6C8B7795C}" parentId="{469B3B8C-9AAA-4F77-A9E0-627E46FBA57E}">
+  <threadedComment ref="E27" dT="2025-03-14T11:42:05.89" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{C7EE2D89-B73E-4A20-A7C5-2FA6C8B7795C}" parentId="{469B3B8C-9AAA-4F77-A9E0-627E46FBA57E}">
     <text>Fontos: GTIN14-et kell megadni</text>
   </threadedComment>
-  <threadedComment ref="D30" dT="2025-03-13T15:56:18.03" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{CB3DD1A3-D70E-42C1-ADB5-EEDBE95CE57C}">
+  <threadedComment ref="E30" dT="2025-03-13T15:56:18.03" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{CB3DD1A3-D70E-42C1-ADB5-EEDBE95CE57C}">
     <text>SAP átállás után ez benne lesz, most nincsen.</text>
   </threadedComment>
-  <threadedComment ref="D33" dT="2025-03-17T08:53:02.39" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{65BEF406-0A3A-492F-B3B3-522C2928A9AB}">
+  <threadedComment ref="E33" dT="2025-03-17T08:53:02.39" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{65BEF406-0A3A-492F-B3B3-522C2928A9AB}">
     <text>Kell?</text>
   </threadedComment>
-  <threadedComment ref="B35" dT="2025-03-17T08:57:39.96" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{6B834A1C-93CE-42EF-B41A-A29ECFCE1F82}">
+  <threadedComment ref="C35" dT="2025-03-17T08:57:39.96" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{6B834A1C-93CE-42EF-B41A-A29ECFCE1F82}">
     <text>Mi a cél?</text>
   </threadedComment>
-  <threadedComment ref="D35" dT="2025-03-17T08:55:32.76" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{07A9BCA0-A72F-45C0-9B30-3977D6F97AFC}">
+  <threadedComment ref="E35" dT="2025-03-17T08:55:32.76" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{07A9BCA0-A72F-45C0-9B30-3977D6F97AFC}">
     <text>Mit adjunk meg? Teljes átmérő.</text>
   </threadedComment>
-  <threadedComment ref="E35" dT="2025-03-14T12:05:50.63" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{29D4DEDB-FEEE-47A0-AAFF-D033EAC89026}">
+  <threadedComment ref="F35" dT="2025-03-14T12:05:50.63" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{29D4DEDB-FEEE-47A0-AAFF-D033EAC89026}">
     <text xml:space="preserve">Additional power (optical)
 Back cylinder axis
 Back cylinder power
@@ -2794,27 +2917,27 @@
 OTHER
 </text>
   </threadedComment>
-  <threadedComment ref="B48" dT="2024-07-22T12:18:48.90" personId="{0520337A-CFA7-4E40-9D95-6AE1712FCF47}" id="{B43E464E-5726-409D-A086-823698CBB3C2}">
+  <threadedComment ref="C48" dT="2024-07-22T12:18:48.90" personId="{0520337A-CFA7-4E40-9D95-6AE1712FCF47}" id="{B43E464E-5726-409D-A086-823698CBB3C2}">
     <text>GS1 kérdés</text>
   </threadedComment>
-  <threadedComment ref="B48" dT="2025-03-07T13:23:44.18" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{8955BACF-29A7-4A24-9E56-B96FE60C00CE}" parentId="{B43E464E-5726-409D-A086-823698CBB3C2}">
+  <threadedComment ref="C48" dT="2025-03-07T13:23:44.18" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{8955BACF-29A7-4A24-9E56-B96FE60C00CE}" parentId="{B43E464E-5726-409D-A086-823698CBB3C2}">
     <text>Lencséknél no, biovis, medjet, jetring</text>
   </threadedComment>
-  <threadedComment ref="B49" dT="2024-07-22T12:21:17.07" personId="{0520337A-CFA7-4E40-9D95-6AE1712FCF47}" id="{9D76ACBD-4553-4AD1-8506-A5BB74A2FDA2}">
+  <threadedComment ref="C49" dT="2024-07-22T12:21:17.07" personId="{0520337A-CFA7-4E40-9D95-6AE1712FCF47}" id="{9D76ACBD-4553-4AD1-8506-A5BB74A2FDA2}">
     <text>Ilyen lesz, nézzünk utána Klinika. Judit!</text>
   </threadedComment>
-  <threadedComment ref="B49" dT="2025-03-13T15:23:20.67" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{169B755B-86E3-4C4A-B487-DAB7C071506D}" parentId="{9D76ACBD-4553-4AD1-8506-A5BB74A2FDA2}">
+  <threadedComment ref="C49" dT="2025-03-13T15:23:20.67" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{169B755B-86E3-4C4A-B487-DAB7C071506D}" parentId="{9D76ACBD-4553-4AD1-8506-A5BB74A2FDA2}">
     <text>PMCF clinical investigation is ide tartozik? Ha nem, akkor nem. Kérdező felület, Eudamed?</text>
   </threadedComment>
-  <threadedComment ref="B54" dT="2024-07-22T12:24:02.85" personId="{0520337A-CFA7-4E40-9D95-6AE1712FCF47}" id="{E14E57AC-D0A2-4625-9716-153B4C796039}">
+  <threadedComment ref="C54" dT="2024-07-22T12:24:02.85" personId="{0520337A-CFA7-4E40-9D95-6AE1712FCF47}" id="{E14E57AC-D0A2-4625-9716-153B4C796039}">
     <text>??? Ezt honnan fogjuk tudni? PMS, PSUR?
 PMCF-ben benne van?
 Kell egy adatbázis</text>
   </threadedComment>
-  <threadedComment ref="B54" dT="2024-07-22T12:25:11.51" personId="{0520337A-CFA7-4E40-9D95-6AE1712FCF47}" id="{B3C4E367-8778-4755-9007-1F66C35C6B25}" parentId="{E14E57AC-D0A2-4625-9716-153B4C796039}">
+  <threadedComment ref="C54" dT="2024-07-22T12:25:11.51" personId="{0520337A-CFA7-4E40-9D95-6AE1712FCF47}" id="{B3C4E367-8778-4755-9007-1F66C35C6B25}" parentId="{E14E57AC-D0A2-4625-9716-153B4C796039}">
     <text>Első CE certification?</text>
   </threadedComment>
-  <threadedComment ref="D55" dT="2025-03-17T09:02:50.50" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{1CD0303A-761E-4078-80D5-AD23DB6AB5DC}">
+  <threadedComment ref="E55" dT="2025-03-17T09:02:50.50" personId="{196B7B68-4976-408E-8C47-F2C854F156FA}" id="{1CD0303A-761E-4078-80D5-AD23DB6AB5DC}">
     <text>Ezt honnan? IT?</text>
   </threadedComment>
 </ThreadedComments>
@@ -2830,666 +2953,731 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D28B0199-4555-45DB-8890-E483BB89FEB6}">
-  <dimension ref="A1:I57"/>
+  <dimension ref="A1:J57"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="25" style="3" customWidth="1"/>
-    <col min="2" max="8" width="31.73046875" style="3" customWidth="1"/>
-    <col min="9" max="9" width="26.73046875" bestFit="1" customWidth="1"/>
+    <col min="1" max="3" width="25" style="3" customWidth="1"/>
+    <col min="4" max="10" width="31.73046875" style="3" customWidth="1"/>
+    <col min="11" max="11" width="26.73046875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="30"/>
+      <c r="C2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A3" s="2"/>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="30" t="s">
+        <v>494</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="E3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="4" spans="1:10" ht="14.65" x14ac:dyDescent="0.5">
       <c r="A4" s="2"/>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="31" t="s">
+        <v>493</v>
+      </c>
+      <c r="C4" s="29" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="E4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="3"/>
-    </row>
-    <row r="5" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="5" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A5" s="2"/>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="30" t="s">
+        <v>513</v>
+      </c>
+      <c r="C5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I5" s="3"/>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E5" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A6" s="2"/>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="30"/>
+      <c r="C6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I6" s="3"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="D6" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="2"/>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="30" t="s">
+        <v>490</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="E7" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    </row>
+    <row r="8" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A8" s="2"/>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="30" t="s">
+        <v>501</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F8" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I8" s="3"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="G8" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="2"/>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="30" t="s">
+        <v>502</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="D9" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E9" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A10" s="2"/>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="30" t="s">
+        <v>503</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="3"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E10" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A11" s="2"/>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="30" t="s">
+        <v>499</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D11" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="3"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E11" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A12" s="2"/>
-      <c r="B12" s="4" t="s">
+      <c r="B12" s="30" t="s">
+        <v>500</v>
+      </c>
+      <c r="C12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="D12" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E12" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A13" s="2"/>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="30" t="s">
+        <v>491</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E13" s="3" t="s">
+      <c r="E13" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F13" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="I13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+    </row>
+    <row r="14" spans="1:10" ht="57" x14ac:dyDescent="0.45">
       <c r="A14" s="2"/>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="30" t="s">
+        <v>492</v>
+      </c>
+      <c r="C14" s="29" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="F14" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="F14" s="9" t="s">
+      <c r="G14" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="I14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A15" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="30"/>
+      <c r="C15" t="s">
         <v>35</v>
       </c>
-      <c r="C15"/>
-      <c r="D15" s="10" t="s">
+      <c r="D15"/>
+      <c r="E15" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
       <c r="H15"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="I15"/>
+      <c r="J15"/>
+    </row>
+    <row r="16" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A16" s="2"/>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="30"/>
+      <c r="C16" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D16" s="14">
+      <c r="E16" s="14">
         <v>2265</v>
       </c>
-      <c r="I16" s="3"/>
-    </row>
-    <row r="17" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="17" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A17" s="2"/>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="30"/>
+      <c r="C17" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="3"/>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E17" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A18" s="2"/>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="30"/>
+      <c r="C18" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="13" t="s">
+      <c r="E18" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="I18" s="3"/>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A19" s="2"/>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="30"/>
+      <c r="C19" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="13" t="s">
+      <c r="E19" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="I19" s="3"/>
-    </row>
-    <row r="20" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="20" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A20" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="30" t="s">
+        <v>505</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="E20" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I20" s="3"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A21" s="2"/>
-      <c r="C21" s="3" t="s">
+      <c r="B21" s="30" t="s">
+        <v>504</v>
+      </c>
+      <c r="D21" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I21" s="3"/>
-    </row>
-    <row r="22" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="22" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A22" s="2"/>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="30"/>
+      <c r="C22" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D22" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="E22" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A23" s="2"/>
-      <c r="B23" s="3" t="s">
+      <c r="B23" s="30" t="s">
+        <v>507</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D23" s="3" t="s">
+      <c r="E23" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="E23" s="5" t="s">
+      <c r="F23" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="F23" s="12" t="s">
+      <c r="G23" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="I23" s="3"/>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A24" s="2"/>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="30" t="s">
+        <v>514</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D24" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E24" s="3" t="s">
+      <c r="E24" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F24" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="F24" s="9" t="s">
+      <c r="G24" s="9" t="s">
         <v>55</v>
       </c>
-      <c r="I24" s="3"/>
-    </row>
-    <row r="25" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="25" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A25" s="2"/>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="30"/>
+      <c r="C25" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="F25" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="F25" s="9" t="s">
+      <c r="G25" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="I25" s="3"/>
-    </row>
-    <row r="26" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="26" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A26" s="2"/>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="30"/>
+      <c r="C26" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="E26" s="3" t="s">
+      <c r="F26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="I26" s="3"/>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="27" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A27" s="2"/>
-      <c r="B27" s="28" t="s">
+      <c r="B27" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="C27" s="28" t="s">
         <v>59</v>
       </c>
-      <c r="D27" s="11" t="s">
+      <c r="E27" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="I27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="28" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A28" s="2"/>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="30"/>
+      <c r="C28" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E28" s="7" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A29" s="2"/>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="30" t="s">
+        <v>515</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D29" s="7">
+      <c r="E29" s="7">
         <v>1</v>
       </c>
-      <c r="I29" s="3"/>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="30" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A30" s="2"/>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="30" t="s">
+        <v>516</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D30" s="8" t="s">
+      <c r="E30" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="I30" s="3"/>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A31" s="2"/>
-      <c r="D31" s="5" t="s">
+      <c r="B31" s="30"/>
+      <c r="E31" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="I31" s="3"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.45">
       <c r="A32" s="2"/>
-      <c r="D32" s="5" t="s">
+      <c r="B32" s="30"/>
+      <c r="E32" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="I32" s="3"/>
-    </row>
-    <row r="33" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="33" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A33" s="2"/>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="30" t="s">
+        <v>517</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D33" s="26" t="s">
+      <c r="E33" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="I33" s="3"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="34" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A34" s="2"/>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="30" t="s">
+        <v>506</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="E34" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="I34" s="3"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A35" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="30"/>
+      <c r="C35" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D35" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I35" s="3"/>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E35" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A36" s="2"/>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="30"/>
+      <c r="C36" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D36" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I36" s="3"/>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E36" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A37" s="2"/>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="30" t="s">
+        <v>510</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="D37" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="3"/>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E37" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A38" s="2"/>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="30" t="s">
+        <v>509</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="D38" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="I38" s="3"/>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E38" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A39" s="2"/>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="30" t="s">
+        <v>511</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="D39" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I39" s="3"/>
-    </row>
-    <row r="40" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+      <c r="E39" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="57" x14ac:dyDescent="0.45">
       <c r="A40" s="2"/>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="30"/>
+      <c r="C40" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="C40" s="3" t="s">
+      <c r="D40" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D40" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I40" s="3"/>
-    </row>
-    <row r="41" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="E40" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A41" s="2"/>
-      <c r="C41" s="3" t="s">
+      <c r="B41" s="30"/>
+      <c r="D41" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D41" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I41" s="3"/>
-    </row>
-    <row r="42" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E41" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A42" s="2"/>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="30" t="s">
+        <v>519</v>
+      </c>
+      <c r="C42" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="D42" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E42" s="3" t="s">
+      <c r="E42" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F42" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="I42" s="3"/>
-    </row>
-    <row r="43" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="43" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A43" s="2"/>
-      <c r="B43" s="29" t="s">
+      <c r="B43" s="30"/>
+      <c r="C43" s="29" t="s">
         <v>79</v>
       </c>
-      <c r="E43" s="3" t="s">
+      <c r="F43" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I43" s="3"/>
-    </row>
-    <row r="44" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="44" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A44" s="2"/>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="30" t="s">
+        <v>518</v>
+      </c>
+      <c r="C44" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="D44" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="E44" s="3" t="s">
+      <c r="E44" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F44" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="I44" s="3"/>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A45" s="2"/>
-      <c r="E45" s="3" t="s">
+      <c r="B45" s="30"/>
+      <c r="F45" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="I45" s="3"/>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="46" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A46" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B46" s="3" t="s">
+      <c r="B46" s="32" t="s">
+        <v>512</v>
+      </c>
+      <c r="C46" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="D46" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I46" s="3"/>
-    </row>
-    <row r="47" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E46" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A47" s="2"/>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="30"/>
+      <c r="C47" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D47" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I47" s="3"/>
-    </row>
-    <row r="48" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="E47" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A48" s="2"/>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="30"/>
+      <c r="C48" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I48" s="3"/>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="E48" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A49" s="2"/>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="30"/>
+      <c r="C49" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D49" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I49" s="3"/>
-    </row>
-    <row r="50" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E49" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A50" s="2"/>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="30" t="s">
+        <v>496</v>
+      </c>
+      <c r="C50" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="D50" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="D50" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I50" s="3"/>
-    </row>
-    <row r="51" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="E50" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A51" s="2"/>
-      <c r="C51" s="3" t="s">
+      <c r="B51" s="30" t="s">
+        <v>495</v>
+      </c>
+      <c r="D51" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="D51" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I51" s="3"/>
-    </row>
-    <row r="52" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="E51" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A52" s="2"/>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="30" t="s">
+        <v>498</v>
+      </c>
+      <c r="C52" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="D52" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="D52" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I52" s="3"/>
-    </row>
-    <row r="53" spans="1:9" ht="57" x14ac:dyDescent="0.45">
+      <c r="E52" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" ht="57" x14ac:dyDescent="0.45">
       <c r="A53" s="2"/>
-      <c r="C53" s="3" t="s">
+      <c r="B53" s="30" t="s">
+        <v>497</v>
+      </c>
+      <c r="D53" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="D53" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="I53" s="3"/>
-    </row>
-    <row r="54" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="E53" s="5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A54" s="2"/>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="30"/>
+      <c r="C54" s="6" t="s">
         <v>95</v>
       </c>
-      <c r="D54" s="3" t="s">
+      <c r="E54" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="I54" s="3"/>
-    </row>
-    <row r="55" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+    </row>
+    <row r="55" spans="1:5" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A55" s="2"/>
-      <c r="B55" s="3" t="s">
+      <c r="B55" s="30"/>
+      <c r="C55" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D55" s="3" t="s">
+      <c r="E55" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="I55" s="3"/>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A56" s="2"/>
-      <c r="D56" s="3" t="s">
+      <c r="B56" s="30"/>
+      <c r="E56" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="I56" s="3"/>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A57" s="2"/>
-      <c r="D57" s="3" t="s">
+      <c r="B57" s="30"/>
+      <c r="E57" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="I57" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F23" r:id="rId1" location="code" display="https://webgate.ec.europa.eu/eudamed/secure - code" xr:uid="{803B10AC-CB63-4EF4-8DE8-65712B6DD19E}"/>
-    <hyperlink ref="D33" r:id="rId2" xr:uid="{ED2518E2-B241-405D-973E-F80EC86B5C41}"/>
+    <hyperlink ref="G23" r:id="rId1" location="code" display="https://webgate.ec.europa.eu/eudamed/secure - code" xr:uid="{803B10AC-CB63-4EF4-8DE8-65712B6DD19E}"/>
+    <hyperlink ref="E33" r:id="rId2" xr:uid="{ED2518E2-B241-405D-973E-F80EC86B5C41}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
@@ -10484,6 +10672,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -10492,7 +10686,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001EF78DA740F76743B5AE001160E051BE" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="93ddf8151dfa6018d176bca93fb55b6c">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1f9fde64-58d4-4c4f-a24e-7a3f1526715c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4a314a2221c82359345bdae72ebed5a3" ns2:_="">
     <xsd:import namespace="1f9fde64-58d4-4c4f-a24e-7a3f1526715c"/>
@@ -10630,13 +10824,23 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31606F28-4595-473E-AED1-D6A3C7D1C745}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="1f9fde64-58d4-4c4f-a24e-7a3f1526715c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52B70F61-3E5F-4E0A-8F63-CFD62C5F1932}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -10644,7 +10848,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A75ACA86-1919-44DB-B10B-56B4758BDD4F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10660,20 +10864,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{31606F28-4595-473E-AED1-D6A3C7D1C745}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="1f9fde64-58d4-4c4f-a24e-7a3f1526715c"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>